<commit_message>
implemented a version to handle stokes parameter input in addition to intensity input and merged into one file before tidying up code
</commit_message>
<xml_diff>
--- a/HWP_hand_low.xlsx
+++ b/HWP_hand_low.xlsx
@@ -10,6 +10,12 @@
     <sheet name="measured" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="calculated" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Adjusted" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Adjusted2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="adjusted3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="adjusted4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="adjusted5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="adjusted6" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="adjusted7" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1521,4 +1527,2590 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01447883819254694</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9796445789548901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006127273473205598</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9599882247915408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05013238617594673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9494310467393855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1837107777623762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9714318683884539</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1381389448659502</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8581223343375272</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3369326505933539</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9825035308492909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2694547670378385</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7274196560540005</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4427264869854463</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9937587120500853</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4250002078531084</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5666668769936601</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4874986332430716</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.977046360984659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6057479357539278</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3862587341913956</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4837101473075963</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9840773846259568</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7492240144805986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2420267170827362</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4146191106315307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9637315694580342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8824533477904921</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1107327273414206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3040872673269749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9759237802318909</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.960232133256255</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03971731814383723</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1601044287309006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9748900712968931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9820552308774912</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01759488173675538</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.01283990189033772</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9650717825182801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9519688006967815</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04803108986764825</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1698379323058297</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9662414295937818</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8620690346708444</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1379310717682178</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3237025842025201</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.97175472713623</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7351021562219855</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.264897620052479</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4190885668640761</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9618163829440505</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5750107083344544</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.424989063485869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4798443797775621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9717542763901136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4020076469829965</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.597991960802552</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.4737149455094483</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9680162326153257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2526688755888427</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7473308541061301</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.4168084469869736</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9698035291497136</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.124382520909913</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8756173796534178</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.3091565863447239</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.973332396819668</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04395104449197721</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9560489207019879</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.1579050479004334</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.965829241392248</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01569307329204831</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9843499412692521</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01028266836270173</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9694025459634443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01447883819254694</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9796445789548901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006127273473205598</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9599882247915408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05013238617594673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9494310467393855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1837107777623762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9714318683884539</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1381389448659502</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8581223343375272</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3369326505933539</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9825035308492909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2694547670378385</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7274196560540005</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4427264869854463</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9937587120500853</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4250002078531084</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5666668769936601</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4874986332430716</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.977046360984659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6057479357539278</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3862587341913956</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4837101473075963</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9840773846259568</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7492240144805986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2420267170827362</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4146191106315307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9637315694580342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8824533477904921</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1107327273414206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3040872673269749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9759237802318909</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.960232133256255</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03971731814383723</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1601044287309006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9748900712968931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9820552308774912</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01759488173675538</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.01283990189033772</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9650717825182801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9519688006967815</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04803108986764825</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1698379323058297</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9662414295937818</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8620690346708444</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1379310717682178</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3237025842025201</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.97175472713623</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7351021562219855</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.264897620052479</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4190885668640761</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9618163829440505</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5750107083344544</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.424989063485869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4798443797775621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9717542763901136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4020076469829965</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.597991960802552</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.4737149455094483</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9680162326153257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2526688755888427</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7473308541061301</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.4168084469869736</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9698035291497136</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.124382520909913</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8756173796534178</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.3091565863447239</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.973332396819668</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04395104449197721</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9560489207019879</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.1579050479004334</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.965829241392248</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01569307329204831</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9843499412692521</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01028266836270173</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9694025459634443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01447883819254694</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9796445789548901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006127273473205598</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9599882247915408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05013238617594673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9494310467393855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1837107777623762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9714318683884539</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1381389448659502</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8581223343375272</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3369326505933539</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9825035308492909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2694547670378385</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7274196560540005</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4427264869854463</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9937587120500853</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4250002078531084</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5666668769936601</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4874986332430716</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.977046360984659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6057479357539278</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3862587341913956</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4837101473075963</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9840773846259568</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7492240144805986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2420267170827362</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4146191106315307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9637315694580342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8824533477904921</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1107327273414206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3040872673269749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9759237802318909</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.960232133256255</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03971731814383723</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1601044287309006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9748900712968931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9820552308774912</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01759488173675538</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.01283990189033772</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9650717825182801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9519688006967815</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04803108986764825</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1698379323058297</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9662414295937818</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8620690346708444</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1379310717682178</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3237025842025201</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.97175472713623</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7351021562219855</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.264897620052479</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4190885668640761</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9618163829440505</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5750107083344544</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.424989063485869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4798443797775621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9717542763901136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4020076469829965</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.597991960802552</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.4737149455094483</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9680162326153257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2526688755888427</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7473308541061301</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.4168084469869736</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9698035291497136</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.124382520909913</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8756173796534178</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.3091565863447239</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.973332396819668</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04395104449197721</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9560489207019879</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.1579050479004334</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.965829241392248</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01569307329204831</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9843499412692521</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01028266836270173</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9694025459634443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01447883819254694</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9796445789548901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006127273473205598</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9599882247915408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05013238617594673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9494310467393855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1837107777623762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9714318683884539</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1381389448659502</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8581223343375272</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3369326505933539</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9825035308492909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2694547670378385</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7274196560540005</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4427264869854463</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9937587120500853</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4250002078531084</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5666668769936601</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4874986332430716</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.977046360984659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6057479357539278</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3862587341913956</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4837101473075963</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9840773846259568</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7492240144805986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2420267170827362</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4146191106315307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9637315694580342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8824533477904921</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1107327273414206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3040872673269749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9759237802318909</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.960232133256255</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03971731814383723</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1601044287309006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9748900712968931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9820552308774912</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01759488173675538</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.01283990189033772</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9650717825182801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9519688006967815</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04803108986764825</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1698379323058297</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9662414295937818</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8620690346708444</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1379310717682178</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3237025842025201</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.97175472713623</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7351021562219855</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.264897620052479</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4190885668640761</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9618163829440505</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5750107083344544</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.424989063485869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4798443797775621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9717542763901136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4020076469829965</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.597991960802552</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.4737149455094483</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9680162326153257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2526688755888427</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7473308541061301</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.4168084469869736</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9698035291497136</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.124382520909913</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8756173796534178</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.3091565863447239</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.973332396819668</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04395104449197721</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9560489207019879</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.1579050479004334</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.965829241392248</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01569307329204831</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9843499412692521</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01028266836270173</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9694025459634443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01447883819254694</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9796445789548901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006127273473205598</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9599882247915408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05013238617594673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9494310467393855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1837107777623762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9714318683884539</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1381389448659502</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8581223343375272</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3369326505933539</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9825035308492909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2694547670378385</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7274196560540005</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4427264869854463</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9937587120500853</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4250002078531084</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5666668769936601</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4874986332430716</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.977046360984659</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6057479357539278</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3862587341913956</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4837101473075963</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9840773846259568</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7492240144805986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2420267170827362</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4146191106315307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9637315694580342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8824533477904921</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1107327273414206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3040872673269749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9759237802318909</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.960232133256255</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03971731814383723</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1601044287309006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9748900712968931</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9820552308774912</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01759488173675538</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.01283990189033772</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9650717825182801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9519688006967815</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04803108986764825</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.1698379323058297</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9662414295937818</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8620690346708444</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1379310717682178</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3237025842025201</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.97175472713623</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7351021562219855</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.264897620052479</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4190885668640761</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9618163829440505</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5750107083344544</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.424989063485869</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4798443797775621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9717542763901136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4020076469829965</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.597991960802552</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.4737149455094483</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9680162326153257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2526688755888427</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7473308541061301</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.4168084469869736</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9698035291497136</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.124382520909913</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8756173796534178</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.3091565863447239</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.973332396819668</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.04395104449197721</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9560489207019879</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.1579050479004334</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.965829241392248</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01569307329204831</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9843499412692521</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01028266836270173</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9694025459634443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.3195222924836676</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3206393792888301</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.002051869727021977</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2049125272834981</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.9034675159553678</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.09643184570695633</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2948625125212926</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9994404558337519</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8588668960046663</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1411171831749043</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3480980188172541</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9999108658489044</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8058766824048178</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1941015347694477</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.395450609743124</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9998750025360679</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.7510161557407167</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2489770661404544</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4324101485835534</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9999719188435741</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6850301308743648</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3149865167659807</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4645401970958261</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.000077975385773</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.6306560010342303</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.3693515910191658</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4826449925477784</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.000039967091766</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5644192654648931</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.4355730194666206</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.4519233245800155</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9167623451141066</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.520685076297183</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.4793010926305875</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3437503496099932</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7371710917894634</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.5090342818256079</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4909472923086059</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2478264359250978</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6229810285855374</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5252165935491433</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4747619387139132</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1734093831417849</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5613929969139881</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.5799888083689571</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.4199884367334678</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.1022501851016595</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5336875055297121</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.68016800799027</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.3198122584092003</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.05502967078391423</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5709649290554171</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8695443779701701</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1304459136266121</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.01751880995197613</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.7737373790456785</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9995067442512144</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0004888638479321785</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0219493592679799</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9999775195360741</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9969315675933181</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.003067119792011062</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.05531334385815304</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.00000108970543</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.9883421651840305</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.01158910433433141</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1064505134405869</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9996179664434587</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.9699762242694037</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.02983870190741427</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1691588664197207</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9989736679562577</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.2923487947039204</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.3093277688880985</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.007140828154850055</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1812534692235981</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>